<commit_message>
changement fait sur : title/description/langue/images
</commit_message>
<xml_diff>
--- a/Rapport_analyse_SEO.xlsx
+++ b/Rapport_analyse_SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\Documents\OPENCLASSROOMS\PROJET_4_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DAB238-282B-45B3-AD58-C63B07A7ABE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F631F00-5976-4FAD-B67F-855559039001}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,8 +388,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +407,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -419,11 +431,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,9 +459,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,10 +474,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -683,7 +701,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -756,63 +774,63 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -931,42 +949,42 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>81</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>59</v>
       </c>
     </row>
@@ -997,7 +1015,7 @@
       <c r="B16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="6" t="s">

</xml_diff>

<commit_message>
modif structure html/ header/navigation
</commit_message>
<xml_diff>
--- a/Rapport_analyse_SEO.xlsx
+++ b/Rapport_analyse_SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\Documents\OPENCLASSROOMS\PROJET_4_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F631F00-5976-4FAD-B67F-855559039001}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BF2525-DDA4-40EC-B6EE-5AA08EB4A519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
   <si>
     <t>Catégorie</t>
   </si>
@@ -234,12 +234,6 @@
     <t>Certains liens vides</t>
   </si>
   <si>
-    <t xml:space="preserve">Rajouter les liens </t>
-  </si>
-  <si>
-    <t>Ajouter les liens des éléments contenant un lien</t>
-  </si>
-  <si>
     <t>https://www.w3.org/TR/WCAG21/#link-purpose-in-context</t>
   </si>
   <si>
@@ -307,13 +301,31 @@
   </si>
   <si>
     <t>Redimensionner les images / Changer le format BMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajouter ou supprimer les liens </t>
+  </si>
+  <si>
+    <t>Ajouter ou supprimer les liens des éléments contenant un lien vide</t>
+  </si>
+  <si>
+    <t>Meta keywords</t>
+  </si>
+  <si>
+    <t>Répétitions des mots clés, non pertinents</t>
+  </si>
+  <si>
+    <t>Enlever les mots clés répétés, revoir la pertinence</t>
+  </si>
+  <si>
+    <t>Mettre des mots clés pertinents, en cohérence avec l'agence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +407,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -436,7 +461,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -481,6 +506,14 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -698,19 +731,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="5" width="82" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="96.33203125" customWidth="1"/>
     <col min="6" max="6" width="140.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -734,23 +767,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -776,39 +809,37 @@
     </row>
     <row r="4" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>31</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>31</v>
@@ -816,42 +847,42 @@
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -859,223 +890,235 @@
         <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>77</v>
       </c>
+      <c r="D14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B15" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="D15" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="8" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="F17" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+    <row r="18" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+    <row r="20" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1084,8 +1127,15 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2064,16 +2114,17 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{9160BDE5-9A43-4D19-A8C6-8EB689B14417}"/>
-    <hyperlink ref="F7" r:id="rId2" location="distinguishable" xr:uid="{C83B0E0D-1C2B-4A9A-A509-BDE0E6BB64FD}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{D481C7EE-919F-444B-B0C8-356844A783B3}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{3EB1270A-B49C-42CE-8187-BBD3C2FA2A99}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{9160BDE5-9A43-4D19-A8C6-8EB689B14417}"/>
+    <hyperlink ref="F8" r:id="rId2" location="distinguishable" xr:uid="{C83B0E0D-1C2B-4A9A-A509-BDE0E6BB64FD}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{D481C7EE-919F-444B-B0C8-356844A783B3}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{3EB1270A-B49C-42CE-8187-BBD3C2FA2A99}"/>
     <hyperlink ref="F2" r:id="rId5" xr:uid="{DF7FAA3C-C227-4032-8FBD-24886499F72B}"/>
     <hyperlink ref="F3" r:id="rId6" xr:uid="{E360C835-ABF2-4E65-8305-6DAE9483A1C8}"/>
-    <hyperlink ref="F13" r:id="rId7" location="optimiser_les_images_dans_une_optique_de_performances" xr:uid="{9712FE88-E370-4896-86B6-807413A20794}"/>
-    <hyperlink ref="F14" r:id="rId8" xr:uid="{9A4E3997-B218-431B-9A74-535A24C1226A}"/>
+    <hyperlink ref="F14" r:id="rId7" location="optimiser_les_images_dans_une_optique_de_performances" xr:uid="{9712FE88-E370-4896-86B6-807413A20794}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{9A4E3997-B218-431B-9A74-535A24C1226A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId9"/>

</xml_diff>